<commit_message>
Add one member in nthu
</commit_message>
<xml_diff>
--- a/AI_expert_list_in_TW.xlsx
+++ b/AI_expert_list_in_TW.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="132" windowWidth="19416" windowHeight="11016"/>
@@ -10,12 +10,12 @@
     <sheet name="工作表2" sheetId="2" r:id="rId1"/>
     <sheet name="工作表3" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="144">
   <si>
     <t>台大</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -229,15 +229,354 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>黃稚存 副教授</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>黃國源 教授</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>陳煥宗 副教授</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>吳尚鴻 副教授</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://www.cs.nthu.edu.tw/~shwu/#research</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://www.cs.nthu.edu.tw/~htchen/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Machine Learning, Big Data Mgm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Networking and Mobile Database Lab</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>陳宜欣 副教授</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://www.cs.nthu.edu.tw/~yishin/research.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Emotion, Intension detection</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Intelligent Data Engineering and Application Lab</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://cymaxwelllee.wixsite.com/elsa</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>本實驗室於2016年二月至九月間，組成研究團隊NVISION，參與NVIDIA公司所主辦之嵌入式智慧型機器人競賽，並獲得全國冠軍的佳績</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>李宏毅 助理教授</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>李濬屹 助理教授</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Robot</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ELSA Lab</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Big Data Analysis, Mental Healthcare</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://www.cs.nthu.edu.tw/~chihya/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>沈之涯 助理教授</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://www.iis.sinica.edu.tw/IASL/hsu/index.html#research</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>智慧型代理人系統實驗室</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>中研院</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>資科</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>許聞廉 所長</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>自然輸入法, 網際網路上的自然語言人機介面，DNA序列分析</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>阮大成 助理教授</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Machine Learning, Data ​Mining​, Energy-Efficient Computing​</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://research.google.com/pubs/DaChengJuan.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Natural Language Processing Lab</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://nlg.csie.ntu.edu.tw/researchdirection.php</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>林守德 教授</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>陳信希 教授</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Web Mining and Information Retrieval Lab</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>林軒田 副教授</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>鄭卜壬 副教授</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Social Listerning</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://www.csie.ntu.edu.tw/~pjcheng/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Big Data Mgm, Data Mining</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://sites.google.com/site/wcpeng/home/projects</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>吳毅成 教授</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Advanced Database System Laboratory</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mobile Data Management, Data Mining, Data Management for Sensor Networks, Databases</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Big Data, Data Mining, Biomedical Informatics, Mobile and Social Networks</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://people.cs.nctu.edu.tw/~vtseng/resch-intst.htm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>彭文志 教授</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>曾新穆 教授</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Big Data and Social Computing Lab</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://bdsc.lab.uic.edu/projects.html</t>
+  </si>
+  <si>
+    <t>Deep learning, Big data, Data Mining</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>俞士綸 教授</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pattern Recognition and Neural Network Computing Lab</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>胡毓志 教授</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bioinformatics, Machine Learning, Data Mining, Artificial Intelligence</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Machine learning, Data Mining</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bioinformatics Lab</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://mapl.nctu.edu.tw/sample/research.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.cs.nctu.edu.tw/cswebsite/members/detail/yhu</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Multimedia Architecture and Processing Lab</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Computer Vision</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cloud Computing and Software Defined Networking, Internet of Things and Big Data Analytics, Energy-aware Mobile Computing and Networking, Dependable Computing and Networks</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.cs.nctu.edu.tw/cswebsite/members/detail/kwang</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mobile Computing and Broadband Networking Lab</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>彭文孝 教授</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>王國禎 教授</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IoT, Big Data</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Computer Games and Intelligence Lab</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Institute of Data Science and Engineering 所長</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>邱維辰 助理教授</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Computer Vision, Machine Learning, Deep Learning, Video Understanding, Generative Models, Nonparametric Bayesian</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://walonchiu.github.io/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Computer Vision, Machine Learning</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Enriched Vision Applications Lab</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Machine Learning Lab</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://chien.cm.nctu.edu.tw/research-area/research-area/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Machine Learning, Deep Learning.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Big Data Mgm, Data Mining, Socail Listerning</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Data Mining, Machine Learning and Mathematical Programming</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Machine Learning, Data Mining</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Data Science and Machine Intelligence Lab</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://www.math.nctu.edu.tw/faculty/faculty_content.php?S_ID=124&amp;SC_ID=1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>簡仁宗 教授</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>李育杰 教授</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>應數</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Machine Learning, Deep Learning</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>許健平 教授</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>黃稚存 副教授</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>黃國源 教授</t>
+    <t>賴尚宏 教授</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -245,346 +584,19 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>陳煥宗 副教授</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>吳尚鴻 副教授</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>http://www.cs.nthu.edu.tw/~shwu/#research</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>http://www.cs.nthu.edu.tw/~htchen/</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Machine Learning, Big Data Mgm</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Networking and Mobile Database Lab</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>陳宜欣 副教授</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>http://www.cs.nthu.edu.tw/~yishin/research.html</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Emotion, Intension detection</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Intelligent Data Engineering and Application Lab</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>http://cymaxwelllee.wixsite.com/elsa</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>本實驗室於2016年二月至九月間，組成研究團隊NVISION，參與NVIDIA公司所主辦之嵌入式智慧型機器人競賽，並獲得全國冠軍的佳績</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>李宏毅 助理教授</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>李濬屹 助理教授</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Robot</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ELSA Lab</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Big Data Analysis, Mental Healthcare</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>http://www.cs.nthu.edu.tw/~chihya/</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>沈之涯 助理教授</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>http://www.iis.sinica.edu.tw/IASL/hsu/index.html#research</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>智慧型代理人系統實驗室</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>中研院</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>資科</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>許聞廉 所長</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>自然輸入法, 網際網路上的自然語言人機介面，DNA序列分析</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>阮大成 助理教授</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Machine Learning, Data ​Mining​, Energy-Efficient Computing​</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://research.google.com/pubs/DaChengJuan.html</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Natural Language Processing Lab</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>http://nlg.csie.ntu.edu.tw/researchdirection.php</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>林守德 教授</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>陳信希 教授</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Web Mining and Information Retrieval Lab</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>林軒田 副教授</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>鄭卜壬 副教授</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Social Listerning</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>http://www.csie.ntu.edu.tw/~pjcheng/</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Big Data Mgm, Data Mining</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://sites.google.com/site/wcpeng/home/projects</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>吳毅成 教授</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Advanced Database System Laboratory</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Mobile Data Management, Data Mining, Data Management for Sensor Networks, Databases</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Big Data, Data Mining, Biomedical Informatics, Mobile and Social Networks</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>http://people.cs.nctu.edu.tw/~vtseng/resch-intst.htm</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>彭文志 教授</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>曾新穆 教授</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Big Data and Social Computing Lab</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>http://bdsc.lab.uic.edu/projects.html</t>
-  </si>
-  <si>
-    <t>Deep learning, Big data, Data Mining</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>俞士綸 教授</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Pattern Recognition and Neural Network Computing Lab</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>胡毓志 教授</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Bioinformatics, Machine Learning, Data Mining, Artificial Intelligence</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Machine learning, Data Mining</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Bioinformatics Lab</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>http://mapl.nctu.edu.tw/sample/research.html</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://www.cs.nctu.edu.tw/cswebsite/members/detail/yhu</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Multimedia Architecture and Processing Lab</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Computer Vision</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Cloud Computing and Software Defined Networking, Internet of Things and Big Data Analytics, Energy-aware Mobile Computing and Networking, Dependable Computing and Networks</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://www.cs.nctu.edu.tw/cswebsite/members/detail/kwang</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Mobile Computing and Broadband Networking Lab</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>彭文孝 教授</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>王國禎 教授</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>IoT, Big Data</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Computer Games and Intelligence Lab</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Institute of Data Science and Engineering 所長</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>邱維辰 助理教授</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Computer Vision, Machine Learning, Deep Learning, Video Understanding, Generative Models, Nonparametric Bayesian</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://walonchiu.github.io/</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Computer Vision, Machine Learning</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Enriched Vision Applications Lab</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Machine Learning Lab</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>http://chien.cm.nctu.edu.tw/research-area/research-area/</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Machine Learning, Deep Learning.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Big Data Mgm, Data Mining, Socail Listerning</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Data Mining, Machine Learning and Mathematical Programming</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Machine Learning, Data Mining</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Data Science and Machine Intelligence Lab</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>http://www.math.nctu.edu.tw/faculty/faculty_content.php?S_ID=124&amp;SC_ID=1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>簡仁宗 教授</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>李育杰 教授</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>應數</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Machine Learning, Deep Learning</t>
+    <t>http://www.cs.nthu.edu.tw/~lai/</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -732,7 +744,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -767,7 +778,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -943,14 +953,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G29"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="16.2"/>
   <cols>
     <col min="1" max="1" width="8.6640625" customWidth="1"/>
     <col min="2" max="2" width="10.88671875" customWidth="1"/>
@@ -961,7 +971,7 @@
     <col min="7" max="7" width="49.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -984,7 +994,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1007,7 +1017,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -1030,7 +1040,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -1038,7 +1048,7 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D4" t="s">
         <v>19</v>
@@ -1053,7 +1063,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -1061,19 +1071,19 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E5" t="s">
         <v>15</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -1081,7 +1091,7 @@
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D6" t="s">
         <v>18</v>
@@ -1096,7 +1106,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -1104,19 +1114,19 @@
         <v>1</v>
       </c>
       <c r="C7" t="s">
+        <v>89</v>
+      </c>
+      <c r="D7" t="s">
+        <v>87</v>
+      </c>
+      <c r="E7" t="s">
+        <v>90</v>
+      </c>
+      <c r="G7" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="D7" t="s">
-        <v>89</v>
-      </c>
-      <c r="E7" t="s">
-        <v>92</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -1139,7 +1149,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -1147,7 +1157,7 @@
         <v>11</v>
       </c>
       <c r="C9" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D9" t="s">
         <v>32</v>
@@ -1162,7 +1172,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7">
       <c r="A10" t="s">
         <v>43</v>
       </c>
@@ -1170,7 +1180,7 @@
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>53</v>
+        <v>139</v>
       </c>
       <c r="D10" t="s">
         <v>45</v>
@@ -1185,7 +1195,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7">
       <c r="A11" t="s">
         <v>43</v>
       </c>
@@ -1193,22 +1203,19 @@
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>54</v>
+        <v>140</v>
       </c>
       <c r="D11" t="s">
-        <v>47</v>
+        <v>142</v>
       </c>
       <c r="E11" t="s">
-        <v>48</v>
-      </c>
-      <c r="F11" t="s">
-        <v>49</v>
+        <v>2</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12" t="s">
         <v>43</v>
       </c>
@@ -1216,19 +1223,19 @@
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D12" t="s">
-        <v>56</v>
+        <v>141</v>
       </c>
       <c r="E12" t="s">
         <v>51</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
       <c r="A13" t="s">
         <v>43</v>
       </c>
@@ -1236,19 +1243,22 @@
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D13" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="E13" t="s">
-        <v>61</v>
+        <v>48</v>
+      </c>
+      <c r="F13" t="s">
+        <v>49</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
       <c r="A14" t="s">
         <v>43</v>
       </c>
@@ -1256,22 +1266,19 @@
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="D14" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="E14" t="s">
-        <v>15</v>
-      </c>
-      <c r="F14" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
       <c r="A15" t="s">
         <v>43</v>
       </c>
@@ -1279,22 +1286,22 @@
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="D15" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="E15" t="s">
-        <v>71</v>
+        <v>15</v>
       </c>
       <c r="F15" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
       <c r="A16" t="s">
         <v>43</v>
       </c>
@@ -1302,16 +1309,22 @@
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>75</v>
+        <v>68</v>
+      </c>
+      <c r="D16" t="s">
+        <v>70</v>
       </c>
       <c r="E16" t="s">
-        <v>73</v>
+        <v>69</v>
+      </c>
+      <c r="F16" t="s">
+        <v>66</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
       <c r="A17" t="s">
         <v>43</v>
       </c>
@@ -1319,39 +1332,33 @@
         <v>1</v>
       </c>
       <c r="C17" t="s">
+        <v>73</v>
+      </c>
+      <c r="E17" t="s">
+        <v>71</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" t="s">
+        <v>43</v>
+      </c>
+      <c r="B18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18" t="s">
+        <v>80</v>
+      </c>
+      <c r="E18" t="s">
+        <v>81</v>
+      </c>
+      <c r="G18" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="E17" t="s">
-        <v>83</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>36</v>
-      </c>
-      <c r="B18" t="s">
-        <v>37</v>
-      </c>
-      <c r="C18" t="s">
-        <v>55</v>
-      </c>
-      <c r="D18" t="s">
-        <v>107</v>
-      </c>
-      <c r="E18" t="s">
-        <v>41</v>
-      </c>
-      <c r="F18" t="s">
-        <v>40</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:7">
       <c r="A19" t="s">
         <v>36</v>
       </c>
@@ -1359,22 +1366,22 @@
         <v>37</v>
       </c>
       <c r="C19" t="s">
-        <v>96</v>
+        <v>54</v>
       </c>
       <c r="D19" t="s">
-        <v>122</v>
+        <v>105</v>
       </c>
       <c r="E19" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="F19" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
       <c r="A20" t="s">
         <v>36</v>
       </c>
@@ -1382,22 +1389,22 @@
         <v>37</v>
       </c>
       <c r="C20" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="D20" t="s">
-        <v>97</v>
+        <v>120</v>
       </c>
       <c r="E20" t="s">
-        <v>132</v>
+        <v>38</v>
       </c>
       <c r="F20" t="s">
-        <v>98</v>
+        <v>38</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
       <c r="A21" t="s">
         <v>36</v>
       </c>
@@ -1405,22 +1412,22 @@
         <v>37</v>
       </c>
       <c r="C21" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D21" t="s">
-        <v>123</v>
+        <v>95</v>
       </c>
       <c r="E21" t="s">
-        <v>94</v>
+        <v>130</v>
       </c>
       <c r="F21" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
       <c r="A22" t="s">
         <v>36</v>
       </c>
@@ -1428,19 +1435,22 @@
         <v>37</v>
       </c>
       <c r="C22" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="D22" t="s">
-        <v>103</v>
+        <v>121</v>
       </c>
       <c r="E22" t="s">
-        <v>105</v>
+        <v>92</v>
+      </c>
+      <c r="F22" t="s">
+        <v>97</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
       <c r="A23" t="s">
         <v>36</v>
       </c>
@@ -1448,22 +1458,19 @@
         <v>37</v>
       </c>
       <c r="C23" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="D23" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="E23" t="s">
-        <v>110</v>
-      </c>
-      <c r="F23" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
       <c r="A24" t="s">
         <v>36</v>
       </c>
@@ -1471,19 +1478,22 @@
         <v>37</v>
       </c>
       <c r="C24" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="D24" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="E24" t="s">
-        <v>115</v>
+        <v>108</v>
+      </c>
+      <c r="F24" t="s">
+        <v>107</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
       <c r="A25" t="s">
         <v>36</v>
       </c>
@@ -1491,22 +1501,19 @@
         <v>37</v>
       </c>
       <c r="C25" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D25" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="E25" t="s">
-        <v>121</v>
-      </c>
-      <c r="F25" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
       <c r="A26" t="s">
         <v>36</v>
       </c>
@@ -1514,88 +1521,111 @@
         <v>37</v>
       </c>
       <c r="C26" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="D26" t="s">
-        <v>128</v>
+        <v>116</v>
       </c>
       <c r="E26" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="F26" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
       <c r="A27" t="s">
         <v>36</v>
       </c>
       <c r="B27" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="C27" t="s">
-        <v>137</v>
+        <v>122</v>
       </c>
       <c r="D27" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="E27" t="s">
-        <v>140</v>
+        <v>125</v>
       </c>
       <c r="F27" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
       <c r="A28" t="s">
         <v>36</v>
       </c>
       <c r="B28" t="s">
-        <v>139</v>
+        <v>11</v>
       </c>
       <c r="C28" t="s">
+        <v>135</v>
+      </c>
+      <c r="D28" t="s">
+        <v>127</v>
+      </c>
+      <c r="E28" t="s">
         <v>138</v>
       </c>
-      <c r="D28" t="s">
-        <v>135</v>
-      </c>
-      <c r="E28" t="s">
+      <c r="F28" t="s">
+        <v>129</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29" t="s">
+        <v>36</v>
+      </c>
+      <c r="B29" t="s">
+        <v>137</v>
+      </c>
+      <c r="C29" t="s">
+        <v>136</v>
+      </c>
+      <c r="D29" t="s">
+        <v>133</v>
+      </c>
+      <c r="E29" t="s">
+        <v>132</v>
+      </c>
+      <c r="F29" t="s">
+        <v>131</v>
+      </c>
+      <c r="G29" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="F28" t="s">
-        <v>133</v>
-      </c>
-      <c r="G28" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30" t="s">
+        <v>76</v>
+      </c>
+      <c r="B30" t="s">
+        <v>77</v>
+      </c>
+      <c r="C30" t="s">
         <v>78</v>
       </c>
-      <c r="B29" t="s">
+      <c r="D30" t="s">
+        <v>75</v>
+      </c>
+      <c r="E30" t="s">
+        <v>15</v>
+      </c>
+      <c r="F30" t="s">
         <v>79</v>
       </c>
-      <c r="C29" t="s">
-        <v>80</v>
-      </c>
-      <c r="D29" t="s">
-        <v>77</v>
-      </c>
-      <c r="E29" t="s">
-        <v>15</v>
-      </c>
-      <c r="F29" t="s">
-        <v>81</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>76</v>
+      <c r="G30" s="1" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -1607,40 +1637,41 @@
     <hyperlink ref="G6" r:id="rId4"/>
     <hyperlink ref="G3" r:id="rId5"/>
     <hyperlink ref="G2" r:id="rId6"/>
-    <hyperlink ref="G19" r:id="rId7" location="achieve"/>
-    <hyperlink ref="G18" r:id="rId8"/>
+    <hyperlink ref="G20" r:id="rId7" location="achieve"/>
+    <hyperlink ref="G19" r:id="rId8"/>
     <hyperlink ref="G10" r:id="rId9"/>
-    <hyperlink ref="G11" r:id="rId10" location="projects"/>
-    <hyperlink ref="G13" r:id="rId11" location="research"/>
+    <hyperlink ref="G13" r:id="rId10" location="projects"/>
+    <hyperlink ref="G14" r:id="rId11" location="research"/>
     <hyperlink ref="G12" r:id="rId12"/>
-    <hyperlink ref="G14" r:id="rId13"/>
-    <hyperlink ref="G15" r:id="rId14"/>
-    <hyperlink ref="G16" r:id="rId15"/>
-    <hyperlink ref="G29" r:id="rId16" location="research"/>
-    <hyperlink ref="G17" r:id="rId17"/>
+    <hyperlink ref="G15" r:id="rId13"/>
+    <hyperlink ref="G16" r:id="rId14"/>
+    <hyperlink ref="G17" r:id="rId15"/>
+    <hyperlink ref="G30" r:id="rId16" location="research"/>
+    <hyperlink ref="G18" r:id="rId17"/>
     <hyperlink ref="G5" r:id="rId18"/>
     <hyperlink ref="G7" r:id="rId19"/>
-    <hyperlink ref="G20" r:id="rId20"/>
-    <hyperlink ref="G21" r:id="rId21"/>
-    <hyperlink ref="G24" r:id="rId22"/>
-    <hyperlink ref="G23" r:id="rId23"/>
-    <hyperlink ref="G25" r:id="rId24"/>
-    <hyperlink ref="G26" r:id="rId25"/>
-    <hyperlink ref="G27" r:id="rId26"/>
-    <hyperlink ref="G28" r:id="rId27"/>
+    <hyperlink ref="G21" r:id="rId20"/>
+    <hyperlink ref="G22" r:id="rId21"/>
+    <hyperlink ref="G25" r:id="rId22"/>
+    <hyperlink ref="G24" r:id="rId23"/>
+    <hyperlink ref="G26" r:id="rId24"/>
+    <hyperlink ref="G27" r:id="rId25"/>
+    <hyperlink ref="G28" r:id="rId26"/>
+    <hyperlink ref="G29" r:id="rId27"/>
+    <hyperlink ref="G11" r:id="rId28"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId28"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId29"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="16.2"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>